<commit_message>
Included all the testcases in the TestNG file
</commit_message>
<xml_diff>
--- a/src/test/java/com/riddhiHousingSociety/testData/TestAddExpense.xlsx
+++ b/src/test/java/com/riddhiHousingSociety/testData/TestAddExpense.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Expense_Done_By</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>06/14/2023</t>
+  </si>
+  <si>
+    <t>06/16/2023</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>10</v>

</xml_diff>